<commit_message>
se unieron las pantallas de maquetas
</commit_message>
<xml_diff>
--- a/Puntos de Funcion.xlsx
+++ b/Puntos de Funcion.xlsx
@@ -196,12 +196,6 @@
     <t>E = 2,17 persona /mes</t>
   </si>
   <si>
-    <t>PUNTOS DE FUNCIÓN NO AJUSTADOS</t>
-  </si>
-  <si>
-    <t>Valores de Ajuste de Complejidad</t>
-  </si>
-  <si>
     <t>LCD</t>
   </si>
   <si>
@@ -241,9 +235,6 @@
     <t>Esfuerzo = 2,17 persona / mes</t>
   </si>
   <si>
-    <t>Cálculo de Esfuerzo</t>
-  </si>
-  <si>
     <t>Fórmulas</t>
   </si>
   <si>
@@ -251,13 +242,22 @@
   </si>
   <si>
     <t>Punto de Función Ajustados</t>
+  </si>
+  <si>
+    <t>Tabla II. Punto de función no ajustados</t>
+  </si>
+  <si>
+    <t>TABLA III. Valores de Ajuste de Complejidad</t>
+  </si>
+  <si>
+    <t>Tabla IV. Cálculo de Esfuerzo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -271,8 +271,27 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -285,8 +304,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="17">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -319,69 +344,20 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -393,66 +369,7 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
+        <color theme="0"/>
       </left>
       <right/>
       <top/>
@@ -460,48 +377,275 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
       </left>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
+      <bottom style="thin">
+        <color theme="0"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="12" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -803,183 +947,197 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="C1" sqref="C1:H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="2.42578125" customWidth="1"/>
     <col min="3" max="3" width="37.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="2.7109375" customWidth="1"/>
+    <col min="9" max="9" width="1.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="5"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="2" t="s">
+    <row r="1" spans="1:9" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="13"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="10"/>
+    </row>
+    <row r="2" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="3"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="5"/>
+    </row>
+    <row r="3" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="3"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="6"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="1" t="s">
+      <c r="H3" s="8"/>
+      <c r="I3" s="5"/>
+    </row>
+    <row r="4" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A4" s="3"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G4" s="23">
         <v>22</v>
       </c>
-      <c r="H4" s="6"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="1" t="s">
+      <c r="H4" s="8"/>
+      <c r="I4" s="5"/>
+    </row>
+    <row r="5" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="3"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="1">
+      <c r="G5" s="23">
         <v>29</v>
       </c>
-      <c r="H5" s="6"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="1" t="s">
+      <c r="H5" s="8"/>
+      <c r="I5" s="5"/>
+    </row>
+    <row r="6" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A6" s="3"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G6" s="23">
         <v>25</v>
       </c>
-      <c r="H6" s="6"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="1" t="s">
+      <c r="H6" s="8"/>
+      <c r="I6" s="5"/>
+    </row>
+    <row r="7" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A7" s="3"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G7" s="23">
         <v>0</v>
       </c>
-      <c r="H7" s="6"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="1" t="s">
+      <c r="H7" s="8"/>
+      <c r="I7" s="5"/>
+    </row>
+    <row r="8" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A8" s="3"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G8" s="23">
         <v>16</v>
       </c>
-      <c r="H8" s="6"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="1">
+      <c r="H8" s="8"/>
+      <c r="I8" s="5"/>
+    </row>
+    <row r="9" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A9" s="3"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="23">
         <f>SUM(G4,G5,G6,G7,G8)</f>
         <v>92</v>
       </c>
-      <c r="H9" s="6"/>
-    </row>
-    <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="6"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="7"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="5"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="5"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H14" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -995,7 +1153,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C1" sqref="C1:E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1003,48 +1161,49 @@
     <col min="2" max="2" width="2.85546875" customWidth="1"/>
     <col min="3" max="3" width="47.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.140625" customWidth="1"/>
+    <col min="5" max="5" width="2.42578125" customWidth="1"/>
     <col min="7" max="7" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="38.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="8"/>
+    <row r="1" spans="1:9" ht="9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3"/>
       <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="5"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="16"/>
-      <c r="C2" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="D2" s="12"/>
-      <c r="E2" s="5"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" s="18"/>
+      <c r="E2" s="16"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="17"/>
+      <c r="B3" s="6"/>
       <c r="C3" s="2" t="s">
         <v>37</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E3" s="6"/>
+      <c r="E3" s="8"/>
       <c r="G3" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="17"/>
+      <c r="B4" s="6"/>
       <c r="C4" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D4" s="1">
         <v>5</v>
       </c>
-      <c r="E4" s="6"/>
+      <c r="E4" s="8"/>
       <c r="G4" t="s">
         <v>39</v>
       </c>
@@ -1053,50 +1212,50 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="17"/>
+      <c r="B5" s="6"/>
       <c r="C5" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D5" s="1">
         <v>2</v>
       </c>
-      <c r="E5" s="6"/>
+      <c r="E5" s="8"/>
       <c r="G5" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="17"/>
+      <c r="B6" s="6"/>
       <c r="C6" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D6" s="1">
         <v>0</v>
       </c>
-      <c r="E6" s="6"/>
+      <c r="E6" s="8"/>
       <c r="G6" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="17"/>
+      <c r="B7" s="6"/>
       <c r="C7" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D7" s="1">
         <v>3</v>
       </c>
-      <c r="E7" s="6"/>
+      <c r="E7" s="8"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="17"/>
+      <c r="B8" s="6"/>
       <c r="C8" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D8" s="1">
         <v>1</v>
       </c>
-      <c r="E8" s="6"/>
+      <c r="E8" s="8"/>
       <c r="G8" t="s">
         <v>45</v>
       </c>
@@ -1105,14 +1264,14 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="17"/>
+      <c r="B9" s="6"/>
       <c r="C9" s="1" t="s">
         <v>28</v>
       </c>
       <c r="D9" s="1">
         <v>1</v>
       </c>
-      <c r="E9" s="6"/>
+      <c r="E9" s="8"/>
       <c r="G9" t="s">
         <v>44</v>
       </c>
@@ -1121,14 +1280,14 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="17"/>
+      <c r="B10" s="6"/>
       <c r="C10" s="1" t="s">
         <v>29</v>
       </c>
       <c r="D10" s="1">
         <v>5</v>
       </c>
-      <c r="E10" s="6"/>
+      <c r="E10" s="8"/>
       <c r="G10" t="s">
         <v>46</v>
       </c>
@@ -1137,95 +1296,95 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="17"/>
+      <c r="B11" s="6"/>
       <c r="C11" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D11" s="1">
         <v>5</v>
       </c>
-      <c r="E11" s="6"/>
+      <c r="E11" s="8"/>
       <c r="G11" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="17"/>
+      <c r="B12" s="6"/>
       <c r="C12" s="1" t="s">
         <v>31</v>
       </c>
       <c r="D12" s="1">
         <v>3</v>
       </c>
-      <c r="E12" s="6"/>
+      <c r="E12" s="8"/>
       <c r="G12" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="17"/>
+      <c r="B13" s="6"/>
       <c r="C13" s="1" t="s">
         <v>32</v>
       </c>
       <c r="D13" s="1">
         <v>3</v>
       </c>
-      <c r="E13" s="6"/>
+      <c r="E13" s="8"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="17"/>
+      <c r="B14" s="6"/>
       <c r="C14" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D14" s="1">
         <v>3</v>
       </c>
-      <c r="E14" s="6"/>
+      <c r="E14" s="8"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="17"/>
+      <c r="B15" s="6"/>
       <c r="C15" s="1" t="s">
         <v>34</v>
       </c>
       <c r="D15" s="1">
         <v>5</v>
       </c>
-      <c r="E15" s="6"/>
+      <c r="E15" s="8"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="17"/>
+      <c r="B16" s="6"/>
       <c r="C16" s="1" t="s">
         <v>35</v>
       </c>
       <c r="D16" s="1">
         <v>3</v>
       </c>
-      <c r="E16" s="6"/>
+      <c r="E16" s="8"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="17"/>
+      <c r="B17" s="6"/>
       <c r="C17" s="1" t="s">
         <v>36</v>
       </c>
       <c r="D17" s="1">
         <v>5</v>
       </c>
-      <c r="E17" s="6"/>
+      <c r="E17" s="8"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="17"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="1">
+      <c r="B18" s="6"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="20">
         <f>SUM(D4:D17)</f>
         <v>44</v>
       </c>
-      <c r="E18" s="6"/>
-    </row>
-    <row r="19" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="18"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="7"/>
+      <c r="E18" s="8"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="9"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1290,128 +1449,141 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G9"/>
+  <dimension ref="B1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="2.85546875" customWidth="1"/>
-    <col min="3" max="3" width="27" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.7109375" customWidth="1"/>
+    <col min="4" max="4" width="57.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="72" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="16"/>
-      <c r="C2" s="12" t="s">
+    <row r="1" spans="2:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+    </row>
+    <row r="2" spans="2:7" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="B2" s="17"/>
+      <c r="C2" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="27"/>
+    </row>
+    <row r="3" spans="2:7" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="B3" s="6"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="31" t="s">
+        <v>72</v>
+      </c>
+      <c r="E3" s="31" t="s">
+        <v>73</v>
+      </c>
+      <c r="F3" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="G3" s="28"/>
+    </row>
+    <row r="4" spans="2:7" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="6"/>
+      <c r="C4" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="33" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="F4" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="G4" s="28"/>
+    </row>
+    <row r="5" spans="2:7" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="6"/>
+      <c r="C5" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="5"/>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="17"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="F3" s="1" t="s">
+      <c r="D5" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="F5" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="G5" s="28"/>
+    </row>
+    <row r="6" spans="2:7" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="6"/>
+      <c r="C6" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="G3" s="6"/>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="17"/>
-      <c r="C4" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E4" s="1" t="s">
+      <c r="E6" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F6" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="G4" s="6"/>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="17"/>
-      <c r="C5" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E5" s="1" t="s">
+      <c r="G6" s="28"/>
+    </row>
+    <row r="7" spans="2:7" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="6"/>
+      <c r="C7" s="35" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7" s="36" t="s">
+        <v>56</v>
+      </c>
+      <c r="E7" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F7" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="G5" s="6"/>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="17"/>
-      <c r="C6" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E6" s="1" t="s">
+      <c r="G7" s="28"/>
+    </row>
+    <row r="8" spans="2:7" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="B8" s="6"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="39"/>
+      <c r="G8" s="40"/>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="9"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="12"/>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="5"/>
+      <c r="G10" s="5"/>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
         <v>71</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G6" s="6"/>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="17"/>
-      <c r="C7" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="G7" s="6"/>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="17"/>
-      <c r="C8" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="6"/>
-    </row>
-    <row r="9" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="18"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>